<commit_message>
Pitch deck to Bappaditya
</commit_message>
<xml_diff>
--- a/ITProjectManagement/Course meterial/InductionDocument.xlsx
+++ b/ITProjectManagement/Course meterial/InductionDocument.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7230" tabRatio="782" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7230" tabRatio="782" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="GCP-GKE" sheetId="9" r:id="rId9"/>
     <sheet name="Jenkins CI" sheetId="5" r:id="rId10"/>
     <sheet name="Sheet2" sheetId="10" r:id="rId11"/>
+    <sheet name="Content" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TrainingRequirements!$A$1:$C$36</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="652">
   <si>
     <t>Anodiam</t>
   </si>
@@ -2045,6 +2046,144 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=Qqx_wzMmFeA</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1bOhCMjUgQNdoAtRPV7y52A-vgaXI1ioV</t>
+  </si>
+  <si>
+    <t>ReactJs</t>
+  </si>
+  <si>
+    <t>ReactNative</t>
+  </si>
+  <si>
+    <t>SpringBoot</t>
+  </si>
+  <si>
+    <t>Tokenizing</t>
+  </si>
+  <si>
+    <t>REST API</t>
+  </si>
+  <si>
+    <t>HTML5</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Katalon</t>
+  </si>
+  <si>
+    <t>GCS</t>
+  </si>
+  <si>
+    <t>GCP MySQL</t>
+  </si>
+  <si>
+    <t>https</t>
+  </si>
+  <si>
+    <t>Database design</t>
+  </si>
+  <si>
+    <t>GKE</t>
+  </si>
+  <si>
+    <t>CICD Jenkins</t>
+  </si>
+  <si>
+    <t>Prometheous</t>
+  </si>
+  <si>
+    <t>Grafana</t>
+  </si>
+  <si>
+    <t>Itsio</t>
+  </si>
+  <si>
+    <t>Load Testing</t>
+  </si>
+  <si>
+    <t>Pen Testing</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Hasicorp Vaults</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Keras</t>
+  </si>
+  <si>
+    <t>Data Viz</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QFaFIcGhPoM&amp;list=PLC3y8-rFHvwgg3vaYJgHGnModB54rxOk3</t>
+  </si>
+  <si>
+    <t>ES6</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=n3zrCxB8sj8&amp;list=PLC3y8-rFHvwhI0V5mE9Vu6Nm-nap8EcjV&amp;index=1</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/11_F1CjnJftkXex2hMz4SET93nyAI_Z2O</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=j942wKiXFu8&amp;list=PL4cUxeGkcC9gZD-Tvwfod2gaISzfRiP9d&amp;index=1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ur6I5m2nTvk&amp;list=PL4cUxeGkcC9ixPU-QkScoRBVxtPPzVjrQ</t>
+  </si>
+  <si>
+    <t>React Project</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Oi4v5uxTY5o&amp;list=PL4cUxeGkcC9iWstfXntcj8f-dFZ4UtlN3</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=esVwR4lGwQE&amp;list=PLLnpHn493BHEqP3gD1pCJYhxX6v2gBZzj</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GLSSRtnNY0g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6RhOzQciVwI&amp;list=PL4cUxeGkcC9hNokByJilPg5g9m2APUePI</t>
+  </si>
+  <si>
+    <t>Context + Hooks</t>
+  </si>
+  <si>
+    <t>React Testing</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZcQyJ-gxke0&amp;list=PL4cUxeGkcC9jx2TTZk3IGWKSbtugYdrlu</t>
+  </si>
+  <si>
+    <t>Async</t>
+  </si>
+  <si>
+    <t>Doodley</t>
+  </si>
+  <si>
+    <t>Speechelo</t>
+  </si>
+  <si>
+    <t>Open Broadcaster Software</t>
+  </si>
+  <si>
+    <t>HTML CSS</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hu-q2zYwEYs&amp;list=PL4cUxeGkcC9ivBf_eKCPIAYXWzLlPAm6G</t>
+  </si>
+  <si>
+    <t>Async Js</t>
   </si>
 </sst>
 </file>
@@ -2317,7 +2456,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2482,6 +2621,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2945,31 +3090,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -3381,6 +3526,40 @@
     <hyperlink ref="C11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="82" t="s">
+        <v>648</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4140,30 +4319,411 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" style="83" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="83">
+        <v>0</v>
+      </c>
+      <c r="E1" s="83" t="s">
+        <v>649</v>
+      </c>
+      <c r="F1" s="83" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>604</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>605</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>604</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="82" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="83"/>
+      <c r="C3" s="15"/>
+      <c r="E3" s="82" t="s">
+        <v>645</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="H3" s="82" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="83"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="80">
+        <v>2</v>
+      </c>
+      <c r="E4" s="80" t="s">
+        <v>632</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C5" s="15" t="s">
+        <v>634</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>607</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>631</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="H5" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="83"/>
+      <c r="C6" s="15"/>
+      <c r="E6" s="81" t="s">
+        <v>642</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="81" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="83"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="81" t="s">
+        <v>637</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="81" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="83"/>
+      <c r="C8" s="15"/>
+      <c r="E8" s="81" t="s">
+        <v>643</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>639</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="81" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="83">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>649</v>
+      </c>
+      <c r="D9" s="80">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>608</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="H9" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="83">
+        <v>2</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>604</v>
+      </c>
+      <c r="D10" s="80">
+        <v>5</v>
+      </c>
+      <c r="E10" s="78" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="83">
+        <v>3</v>
+      </c>
+      <c r="B11" s="83" t="s">
+        <v>651</v>
+      </c>
+      <c r="C11" s="83" t="s">
+        <v>644</v>
+      </c>
+      <c r="D11" s="80">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="83">
+        <v>4</v>
+      </c>
+      <c r="B12" s="83" t="s">
+        <v>632</v>
+      </c>
+      <c r="D12" s="80">
+        <v>7</v>
+      </c>
+      <c r="E12" s="78" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="83">
+        <v>5</v>
+      </c>
+      <c r="B13" s="83" t="s">
+        <v>607</v>
+      </c>
+      <c r="D13" s="80">
+        <v>8</v>
+      </c>
+      <c r="E13" s="78" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="83">
+        <v>6</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>642</v>
+      </c>
+      <c r="D14" s="80">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="83">
+        <v>7</v>
+      </c>
+      <c r="B15" s="83" t="s">
+        <v>637</v>
+      </c>
+      <c r="D15" s="80">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="83">
+        <v>8</v>
+      </c>
+      <c r="B16" s="83" t="s">
+        <v>643</v>
+      </c>
+      <c r="D16" s="80">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="83">
+        <v>9</v>
+      </c>
+      <c r="B17" s="83" t="s">
+        <v>608</v>
+      </c>
+      <c r="D17" s="80">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="80">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="80">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D20" s="80">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="80">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="80">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="80">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="83"/>
+      <c r="D24" s="80">
+        <v>19</v>
+      </c>
+      <c r="E24" s="79" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="80">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="80">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="80">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="80">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="80">
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="80">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="80">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D32" s="80">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" s="80">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" s="80">
+        <v>29</v>
+      </c>
+      <c r="E34" t="s">
+        <v>630</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -9590,13 +10150,13 @@
       <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="3" spans="1:5" s="33" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="55"/>
@@ -10391,13 +10951,13 @@
       <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" s="51" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="89" t="s">
         <v>425</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="3" spans="1:5" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="55"/>

</xml_diff>